<commit_message>
Various script updates to fix bugs
</commit_message>
<xml_diff>
--- a/Netsuite_Active_Leases.xlsx
+++ b/Netsuite_Active_Leases.xlsx
@@ -1977,19 +1977,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.3" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.90625" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" style="4"/>
-    <col min="8" max="9" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.7265625" style="4"/>
+    <col min="5" max="5" width="6.90625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="43.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="60.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.36328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.90625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>